<commit_message>
Contiue with Udacity Inferential Stats, Udemy SQL, and GATech Modeling, start UT Data Analysis 2 and UCSD Python for Data Science
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson6_t_Test_pt3.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson6_t_Test_pt3.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="food" sheetId="1" r:id="rId1"/>
     <sheet name="pooled variance" sheetId="2" r:id="rId2"/>
+    <sheet name="problem set" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
   <si>
     <t>A</t>
   </si>
@@ -244,6 +245,111 @@
   </si>
   <si>
     <t>dF(xy)</t>
+  </si>
+  <si>
+    <t>df(n)</t>
+  </si>
+  <si>
+    <t>df(p)</t>
+  </si>
+  <si>
+    <t>^ then take square root of the sum of pooled variance divided by each n --&gt; sqrt(SE(p)^2/n1 + SE(p)^2/n2))</t>
+  </si>
+  <si>
+    <t>&lt;-- mean difference / corrected SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha </t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>&lt;-- CARE ABOUT DIRECTION = ONE-TAIL</t>
+  </si>
+  <si>
+    <t>&lt;-- DON’T CARE ABOUT DIRECTION, JUST IF DIFFERENT = TWO-TAIL</t>
+  </si>
+  <si>
+    <t>&lt;-- pooled variance &lt;-- get from sum of Sum of Squared Errors (SS or SSE) of x + y divided by dF of x y = [SS(x)+SS(y)]/[dF(x)+dF(y)]</t>
+  </si>
+  <si>
+    <t>S(p)^2</t>
+  </si>
+  <si>
+    <t>SE©</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE(c) </t>
+  </si>
+  <si>
+    <t>&lt;-- w/in critical region = reject null</t>
+  </si>
+  <si>
+    <t>+/- 1.684</t>
+  </si>
+  <si>
+    <t>+/- 1.984</t>
+  </si>
+  <si>
+    <t>+/- 2.626</t>
+  </si>
+  <si>
+    <t>&lt;-- use from dF = 100 b/c closest</t>
+  </si>
+  <si>
+    <t>x edv's</t>
+  </si>
+  <si>
+    <t>x dev's^2</t>
+  </si>
+  <si>
+    <t>y dev's</t>
+  </si>
+  <si>
+    <t>y dev's ^2</t>
+  </si>
+  <si>
+    <t>x(x)</t>
+  </si>
+  <si>
+    <t>x(y)</t>
+  </si>
+  <si>
+    <t>dF(x)</t>
+  </si>
+  <si>
+    <t>dF(y)</t>
+  </si>
+  <si>
+    <t>y(y)</t>
+  </si>
+  <si>
+    <t>dF©</t>
+  </si>
+  <si>
+    <t>+-/3.499</t>
+  </si>
+  <si>
+    <t>&lt;- Reject null</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>S(p)</t>
+  </si>
+  <si>
+    <t>Cohen's d</t>
+  </si>
+  <si>
+    <t>&lt;--- how many SD's apart</t>
+  </si>
+  <si>
+    <t>&lt;-- % of variability due to IV</t>
   </si>
 </sst>
 </file>
@@ -345,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,13 +464,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,6 +560,125 @@
         <a:xfrm>
           <a:off x="11477625" y="6315075"/>
           <a:ext cx="1028571" cy="695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="0"/>
+          <a:ext cx="1438275" cy="711176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>363566</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>456892</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1678016" y="2752725"/>
+          <a:ext cx="1312526" cy="866571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>183424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>49054</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429750" y="2469424"/>
+          <a:ext cx="1428750" cy="627630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -757,10 +984,10 @@
         <f>AVERAGE(A2:A8)</f>
         <v>20.228571428571428</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6"/>
+      <c r="I1" s="10"/>
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1721,7 @@
       <c r="P37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q37" s="7" t="s">
+      <c r="Q37" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1544,22 +1771,22 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M43" s="8" t="s">
+      <c r="M43" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M44" s="8" t="s">
+      <c r="M44" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M45" s="9" t="s">
+      <c r="M45" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M46" s="9" t="s">
+      <c r="M46" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1577,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1981,7 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1765,7 +1992,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1776,7 +2003,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K9" t="s">
@@ -1800,4 +2027,700 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>3.8</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="2">
+        <f>SQRT(B6/B4+B6/B5)</f>
+        <v>0.11145502331533659</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B4-1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="2">
+        <f>B5-1</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="2">
+        <f>SUM(B8:B9)-2</f>
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="11">
+        <f>(B2-B3)/B7</f>
+        <v>15.252789416141766</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15">
+        <v>0.05</v>
+      </c>
+      <c r="N15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N16" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="N17" t="s">
+        <v>78</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="N18" t="s">
+        <v>70</v>
+      </c>
+      <c r="O18">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19">
+        <v>52</v>
+      </c>
+      <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s">
+        <v>62</v>
+      </c>
+      <c r="O20">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="N21" t="s">
+        <v>63</v>
+      </c>
+      <c r="O21">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2">
+        <f>SQRT(B21/B19+B21/B20)</f>
+        <v>0.43307113421174748</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O22" s="2">
+        <f>SUM(O20:O21)/SUM(O24:O25)</f>
+        <v>1.8894117647058823</v>
+      </c>
+      <c r="R22">
+        <f>(33.14-18)/15.72</f>
+        <v>0.96310432569974558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="2">
+        <f>B19-1</f>
+        <v>51</v>
+      </c>
+      <c r="E23">
+        <f>(33.14-18)/15.72</f>
+        <v>0.96310432569974558</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" s="2">
+        <f>SQRT(O22/O18+O22/O19)</f>
+        <v>0.13310082028421025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2">
+        <f>B20-1</f>
+        <v>56</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O24" s="2">
+        <f>O18-1</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="2">
+        <f>SUM(B19:B20)-2</f>
+        <v>107</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O25" s="2">
+        <f>O19-1</f>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O26" s="2">
+        <f>SUM(O18:O19)-2</f>
+        <v>425</v>
+      </c>
+      <c r="P26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2">
+        <f>((B16-B17)-B18)/B22</f>
+        <v>2.3090894797690584</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="P27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" s="2">
+        <f>((O15-O16)-O17)/O23</f>
+        <v>31.555027166862935</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <f>A33-$B$38</f>
+        <v>-1</v>
+      </c>
+      <c r="C33">
+        <f>B33^2</f>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <f>D33-$E$38</f>
+        <v>-2</v>
+      </c>
+      <c r="F33">
+        <f>E33^2</f>
+        <v>4</v>
+      </c>
+      <c r="H33" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33">
+        <f>COUNT(B33:B37)</f>
+        <v>5</v>
+      </c>
+      <c r="M33" t="s">
+        <v>99</v>
+      </c>
+      <c r="N33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-3</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:B37" si="0">A34-$B$38</f>
+        <v>-6</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:C37" si="1">B34^2</f>
+        <v>36</v>
+      </c>
+      <c r="D34">
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E36" si="2">D34-$E$38</f>
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F36" si="3">E34^2</f>
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34">
+        <f>COUNT(D33:D36)</f>
+        <v>4</v>
+      </c>
+      <c r="M34" t="s">
+        <v>20</v>
+      </c>
+      <c r="N34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="H35" t="s">
+        <v>96</v>
+      </c>
+      <c r="I35">
+        <f>I33-1</f>
+        <v>4</v>
+      </c>
+      <c r="M35" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36">
+        <f>I34-1</f>
+        <v>3</v>
+      </c>
+      <c r="M36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36">
+        <v>2.101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="H37" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37">
+        <f>SUM(I33:I34)-2</f>
+        <v>7</v>
+      </c>
+      <c r="M37" t="s">
+        <v>102</v>
+      </c>
+      <c r="N37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="2">
+        <f>AVERAGE(A33:A37)</f>
+        <v>3</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="2">
+        <f>AVERAGE(D33:D36)</f>
+        <v>12</v>
+      </c>
+      <c r="M38" t="s">
+        <v>103</v>
+      </c>
+      <c r="N38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="2">
+        <f>SUM(C33:C37)</f>
+        <v>58</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="2">
+        <f>SUM(F33:F37)</f>
+        <v>18</v>
+      </c>
+      <c r="M39" t="s">
+        <v>6</v>
+      </c>
+      <c r="N39">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="2">
+        <f>((B39+E39)/(I35+I36))</f>
+        <v>10.857142857142858</v>
+      </c>
+      <c r="M40" t="s">
+        <v>19</v>
+      </c>
+      <c r="N40">
+        <f>(N37-N38)/N39</f>
+        <v>3.191489361702128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2">
+        <f>SQRT(B40/I33+B40/I34)</f>
+        <v>2.210365192839022</v>
+      </c>
+      <c r="M41" t="s">
+        <v>104</v>
+      </c>
+      <c r="N41">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="2">
+        <f>(B38-E38)/B41</f>
+        <v>-4.0717253552297761</v>
+      </c>
+      <c r="M42" t="s">
+        <v>105</v>
+      </c>
+      <c r="N42">
+        <f>(N37-N38)/N41</f>
+        <v>1.2875536480686696</v>
+      </c>
+      <c r="O42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>0.01</v>
+      </c>
+      <c r="M43" t="s">
+        <v>53</v>
+      </c>
+      <c r="N43">
+        <f>(N40^2/(N40^2+N33))*100</f>
+        <v>36.137612026597289</v>
+      </c>
+      <c r="O43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>